<commit_message>
add modifications after validation with the responsible
- add automatic filled column : due date in tabel problem_descriptions (equals claim->opening_date +1 day)
-change options of column bontaz_plant in label_checkings table
- edit the column scrap in sortings table to an auto column wich equals : qty_NOK/qty_sorted * 100
- add column hour in meetings table
</commit_message>
<xml_diff>
--- a/storage/Bontaz_copy.xlsx
+++ b/storage/Bontaz_copy.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="287">
   <si>
     <t>QRQC Report &amp; Simplified 8D</t>
   </si>
@@ -259,13 +259,13 @@
     <t>8D REFERENCE (Bontaz)</t>
   </si>
   <si>
-    <t>C5265439</t>
+    <t>hugy86</t>
   </si>
   <si>
-    <t>B8569317</t>
+    <t>ugytfyh45</t>
   </si>
   <si>
-    <t>2023-06-04</t>
+    <t>2023-07-18</t>
   </si>
   <si>
     <t>Product / Process / System</t>
@@ -291,10 +291,10 @@
     </r>
   </si>
   <si>
-    <t>GIC24</t>
+    <t>BOB65</t>
   </si>
   <si>
-    <t>2023-07-13 14:13:28</t>
+    <t>2023-07-18 16:27:29</t>
   </si>
   <si>
     <t>2. PROBLEM DESCRIPTION</t>
@@ -318,8 +318,8 @@
     <t>Traceability :</t>
   </si>
   <si>
-    <t>Engraving : 4362154 
- Production date : 2023-06-08</t>
+    <t>Engraving : 458 
+ Production date : 2023-06-28</t>
   </si>
   <si>
     <t>Reccurence ?</t>
@@ -388,6 +388,18 @@
     <t xml:space="preserve">Potential actions  (Help): </t>
   </si>
   <si>
+    <t>rrrrrrrrrrrrrrrrrrrrr</t>
+  </si>
+  <si>
+    <t>YASSINE</t>
+  </si>
+  <si>
+    <t>2023-07-20</t>
+  </si>
+  <si>
+    <t>on going</t>
+  </si>
+  <si>
     <t>- Detailled remedial measure for the cause of the defect</t>
   </si>
   <si>
@@ -409,6 +421,15 @@
     <t xml:space="preserve">Implemented actions  (Help): </t>
   </si>
   <si>
+    <t>iiiiiiiiiiiiii</t>
+  </si>
+  <si>
+    <t>2023-07-21</t>
+  </si>
+  <si>
+    <t>not started</t>
+  </si>
+  <si>
     <t>- Detailled description of measure on occurrence and detection (scope of testing, result, update of document or method, …)</t>
   </si>
   <si>
@@ -416,6 +437,12 @@
   </si>
   <si>
     <t xml:space="preserve">Preventive actions  (Help): </t>
+  </si>
+  <si>
+    <t>ooooooooooo</t>
+  </si>
+  <si>
+    <t>Chaymaa Mouwahid</t>
   </si>
   <si>
     <t>- Measure taken so the cause of the defect does not occur on another product, process or system (initial part release process, lesson learned, monitoring of parameters, …)</t>
@@ -470,6 +497,9 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Chaymaa.Mouwahid@bontaz.com</t>
+  </si>
+  <si>
     <t>PRESENCE CHECK LIST</t>
   </si>
   <si>
@@ -497,6 +527,12 @@
     <t>Sign</t>
   </si>
   <si>
+    <t>Customer Quality Responsible</t>
+  </si>
+  <si>
+    <t>Stagiaire</t>
+  </si>
+  <si>
     <t>PROBLEM DESCRIPTION</t>
   </si>
   <si>
@@ -518,6 +554,9 @@
   </si>
   <si>
     <t>Date of reception :</t>
+  </si>
+  <si>
+    <t>2023-08-01</t>
   </si>
   <si>
     <t>6. BONTAZ FAULT</t>
@@ -547,7 +586,13 @@
     <t>Sorting method</t>
   </si>
   <si>
+    <t>tri</t>
+  </si>
+  <si>
     <t>BONTAZ Plant</t>
+  </si>
+  <si>
+    <t>Troy</t>
   </si>
   <si>
     <t>CONTAINMENT LIST - RISK ASSESMENT</t>
@@ -564,7 +609,7 @@
     <t>Update date</t>
   </si>
   <si>
-    <t>2023-07-12 12:33:47</t>
+    <t>2023-07-18 16:19:34</t>
   </si>
   <si>
     <t>SORTING METHOD</t>
@@ -951,21 +996,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>skjfdsqfn sfkjshfjsqhfuy hffusqf</t>
-  </si>
-  <si>
-    <t>qqqqqqqqqq</t>
-  </si>
-  <si>
-    <t>ffff</t>
-  </si>
-  <si>
-    <t>ooooooooooooo</t>
-  </si>
-  <si>
-    <t>iiiii</t>
   </si>
   <si>
     <t>Measurement</t>
@@ -4160,6 +4190,66 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="809625" cy="762000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1524000" cy="762000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
@@ -4798,6 +4888,66 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="914400" cy="857250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1714500" cy="857250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
@@ -5333,7 +5483,7 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="857250" cy="857250"/>
+    <xdr:ext cx="1714500" cy="857250"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="8" name="" descr=""/>
@@ -5363,7 +5513,7 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="857250" cy="857250"/>
+    <xdr:ext cx="1714500" cy="857250"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="9" name="" descr=""/>
@@ -5393,7 +5543,7 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="857250" cy="857250"/>
+    <xdr:ext cx="1714500" cy="857250"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="10" name="" descr=""/>
@@ -5423,7 +5573,7 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="857250" cy="857250"/>
+    <xdr:ext cx="1714500" cy="857250"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="11" name="" descr=""/>
@@ -7663,7 +7813,7 @@
       <c r="B2" s="11"/>
       <c r="C2" s="4"/>
       <c r="D2" s="252" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="E2" s="252"/>
       <c r="F2" s="252"/>
@@ -7673,7 +7823,7 @@
       <c r="J2" s="252"/>
       <c r="K2" s="252"/>
       <c r="L2" s="253" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="M2" s="253"/>
       <c r="N2" s="10"/>
@@ -7713,21 +7863,21 @@
     <row r="5" spans="1:18" customHeight="1" ht="15">
       <c r="A5" s="10"/>
       <c r="B5" s="235" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C5" s="236"/>
       <c r="D5" s="236"/>
       <c r="E5" s="236"/>
       <c r="F5" s="237"/>
       <c r="G5" s="235" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="H5" s="236"/>
       <c r="I5" s="236"/>
       <c r="J5" s="236"/>
       <c r="K5" s="237"/>
       <c r="L5" s="235" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="M5" s="237"/>
       <c r="N5" s="10"/>
@@ -7742,13 +7892,15 @@
       <c r="E6" s="248"/>
       <c r="F6" s="249"/>
       <c r="G6" s="247">
-        <v>8563214</v>
+        <v>856491</v>
       </c>
       <c r="H6" s="248"/>
       <c r="I6" s="248"/>
       <c r="J6" s="248"/>
       <c r="K6" s="249"/>
-      <c r="L6" s="250"/>
+      <c r="L6" s="250" t="s">
+        <v>170</v>
+      </c>
       <c r="M6" s="251"/>
       <c r="N6" s="10"/>
     </row>
@@ -7772,7 +7924,7 @@
     <row r="8" spans="1:18" customHeight="1" ht="15">
       <c r="A8" s="13"/>
       <c r="B8" s="230" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="C8" s="231"/>
       <c r="D8" s="231"/>
@@ -7788,7 +7940,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="31"/>
       <c r="P8" s="49" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="Q8" s="29"/>
       <c r="R8" s="49"/>
@@ -7810,7 +7962,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="31"/>
       <c r="P9" s="48" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="Q9" s="29"/>
       <c r="R9" s="48"/>
@@ -9777,7 +9929,7 @@
       <c r="L16" s="159"/>
       <c r="M16" s="159"/>
       <c r="N16" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="30"/>
@@ -10387,7 +10539,9 @@
     </row>
     <row r="39" spans="1:24" customHeight="1" ht="15">
       <c r="A39" s="13"/>
-      <c r="B39" s="258"/>
+      <c r="B39" s="258" t="s">
+        <v>99</v>
+      </c>
       <c r="C39" s="259"/>
       <c r="D39" s="259"/>
       <c r="E39" s="259"/>
@@ -10397,13 +10551,19 @@
       <c r="I39" s="259"/>
       <c r="J39" s="259"/>
       <c r="K39" s="260"/>
-      <c r="L39" s="123"/>
-      <c r="M39" s="123"/>
-      <c r="N39" s="123"/>
+      <c r="L39" s="123" t="s">
+        <v>100</v>
+      </c>
+      <c r="M39" s="123" t="s">
+        <v>101</v>
+      </c>
+      <c r="N39" s="123" t="s">
+        <v>102</v>
+      </c>
       <c r="O39" s="3"/>
       <c r="P39" s="30"/>
       <c r="Q39" s="48" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="R39" s="30"/>
       <c r="S39" s="30"/>
@@ -10430,7 +10590,7 @@
       <c r="O40" s="3"/>
       <c r="P40" s="30"/>
       <c r="Q40" s="48" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="R40" s="30"/>
       <c r="S40" s="30"/>
@@ -10517,14 +10677,14 @@
     <row r="44" spans="1:24" customHeight="1" ht="15">
       <c r="A44" s="13"/>
       <c r="B44" s="158" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C44" s="159"/>
       <c r="D44" s="22">
         <v>0</v>
       </c>
       <c r="E44" s="158" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F44" s="159"/>
       <c r="G44" s="160"/>
@@ -10577,7 +10737,7 @@
     <row r="46" spans="1:24" customHeight="1" ht="15">
       <c r="A46" s="13"/>
       <c r="B46" s="165" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C46" s="166"/>
       <c r="D46" s="166"/>
@@ -10592,7 +10752,7 @@
         <v>95</v>
       </c>
       <c r="M46" s="122" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="N46" s="122" t="s">
         <v>97</v>
@@ -10600,7 +10760,7 @@
       <c r="O46" s="3"/>
       <c r="P46" s="30"/>
       <c r="Q46" s="49" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="R46" s="30"/>
       <c r="S46" s="30"/>
@@ -10611,7 +10771,9 @@
     </row>
     <row r="47" spans="1:24" customHeight="1" ht="15">
       <c r="A47" s="13"/>
-      <c r="B47" s="255"/>
+      <c r="B47" s="255" t="s">
+        <v>110</v>
+      </c>
       <c r="C47" s="255"/>
       <c r="D47" s="255"/>
       <c r="E47" s="255"/>
@@ -10621,13 +10783,19 @@
       <c r="I47" s="255"/>
       <c r="J47" s="255"/>
       <c r="K47" s="255"/>
-      <c r="L47" s="123"/>
-      <c r="M47" s="123"/>
-      <c r="N47" s="123"/>
+      <c r="L47" s="123" t="s">
+        <v>100</v>
+      </c>
+      <c r="M47" s="123" t="s">
+        <v>111</v>
+      </c>
+      <c r="N47" s="123" t="s">
+        <v>112</v>
+      </c>
       <c r="O47" s="3"/>
       <c r="P47" s="30"/>
       <c r="Q47" s="48" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="R47" s="30"/>
       <c r="S47" s="30"/>
@@ -10766,7 +10934,7 @@
     <row r="53" spans="1:24" customHeight="1" ht="15">
       <c r="A53" s="13"/>
       <c r="B53" s="165" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C53" s="166"/>
       <c r="D53" s="166"/>
@@ -10781,7 +10949,7 @@
         <v>95</v>
       </c>
       <c r="M53" s="122" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="N53" s="122" t="s">
         <v>97</v>
@@ -10789,7 +10957,7 @@
       <c r="O53" s="3"/>
       <c r="P53" s="30"/>
       <c r="Q53" s="49" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="R53" s="30"/>
       <c r="S53" s="30"/>
@@ -10800,7 +10968,9 @@
     </row>
     <row r="54" spans="1:24" customHeight="1" ht="15">
       <c r="A54" s="13"/>
-      <c r="B54" s="255"/>
+      <c r="B54" s="255" t="s">
+        <v>116</v>
+      </c>
       <c r="C54" s="255"/>
       <c r="D54" s="255"/>
       <c r="E54" s="255"/>
@@ -10810,13 +10980,19 @@
       <c r="I54" s="255"/>
       <c r="J54" s="255"/>
       <c r="K54" s="255"/>
-      <c r="L54" s="123"/>
-      <c r="M54" s="123"/>
-      <c r="N54" s="123"/>
+      <c r="L54" s="123" t="s">
+        <v>117</v>
+      </c>
+      <c r="M54" s="123" t="s">
+        <v>101</v>
+      </c>
+      <c r="N54" s="123" t="s">
+        <v>112</v>
+      </c>
       <c r="O54" s="3"/>
       <c r="P54" s="30"/>
       <c r="Q54" s="48" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="R54" s="30"/>
       <c r="S54" s="30"/>
@@ -10843,7 +11019,7 @@
       <c r="O55" s="3"/>
       <c r="P55" s="30"/>
       <c r="Q55" s="48" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="R55" s="30"/>
       <c r="S55" s="30"/>
@@ -10880,28 +11056,28 @@
     <row r="57" spans="1:24" customHeight="1" ht="15">
       <c r="A57" s="13"/>
       <c r="B57" s="158" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C57" s="159"/>
       <c r="D57" s="22">
         <v>0</v>
       </c>
       <c r="E57" s="158" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="F57" s="159"/>
       <c r="G57" s="22">
         <v>0</v>
       </c>
       <c r="H57" s="158" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="I57" s="159"/>
       <c r="J57" s="22">
         <v>0</v>
       </c>
       <c r="K57" s="158" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="L57" s="159"/>
       <c r="M57" s="124">
@@ -11613,7 +11789,7 @@
       <c r="B2" s="11"/>
       <c r="C2" s="4"/>
       <c r="D2" s="252" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="E2" s="252"/>
       <c r="F2" s="252"/>
@@ -11623,7 +11799,7 @@
       <c r="J2" s="252"/>
       <c r="K2" s="252"/>
       <c r="L2" s="253" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="M2" s="253"/>
       <c r="N2" s="10"/>
@@ -11720,7 +11896,7 @@
     <row r="8" spans="1:18" customHeight="1" ht="15">
       <c r="A8" s="11"/>
       <c r="B8" s="277" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C8" s="278"/>
       <c r="D8" s="278"/>
@@ -13237,7 +13413,7 @@
       <c r="B2" s="11"/>
       <c r="C2" s="4"/>
       <c r="D2" s="252" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="E2" s="252"/>
       <c r="F2" s="252"/>
@@ -13247,7 +13423,7 @@
       <c r="J2" s="252"/>
       <c r="K2" s="252"/>
       <c r="L2" s="253" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="M2" s="253"/>
       <c r="N2" s="10"/>
@@ -13287,14 +13463,14 @@
     <row r="5" spans="1:18" customHeight="1" ht="15" s="31" customFormat="1">
       <c r="A5" s="5"/>
       <c r="B5" s="235" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C5" s="236"/>
       <c r="D5" s="236"/>
       <c r="E5" s="236"/>
       <c r="F5" s="237"/>
       <c r="G5" s="235" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="H5" s="236"/>
       <c r="I5" s="236"/>
@@ -13348,19 +13524,19 @@
     <row r="8" spans="1:18" customHeight="1" ht="15" s="31" customFormat="1">
       <c r="A8" s="5"/>
       <c r="B8" s="235" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C8" s="236"/>
       <c r="D8" s="236"/>
       <c r="E8" s="236"/>
       <c r="F8" s="237"/>
       <c r="G8" s="235" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="H8" s="236"/>
       <c r="I8" s="236"/>
       <c r="J8" s="235" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="K8" s="236"/>
       <c r="L8" s="236"/>
@@ -13369,7 +13545,9 @@
     </row>
     <row r="9" spans="1:18" customHeight="1" ht="15">
       <c r="A9" s="13"/>
-      <c r="B9" s="247"/>
+      <c r="B9" s="247" t="s">
+        <v>117</v>
+      </c>
       <c r="C9" s="248"/>
       <c r="D9" s="248"/>
       <c r="E9" s="248"/>
@@ -13377,7 +13555,9 @@
       <c r="G9" s="247"/>
       <c r="H9" s="248"/>
       <c r="I9" s="248"/>
-      <c r="J9" s="247"/>
+      <c r="J9" s="247" t="s">
+        <v>134</v>
+      </c>
       <c r="K9" s="248"/>
       <c r="L9" s="248"/>
       <c r="M9" s="249"/>
@@ -13404,7 +13584,7 @@
     <row r="11" spans="1:18" customHeight="1" ht="15">
       <c r="A11" s="13"/>
       <c r="B11" s="303" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="C11" s="304"/>
       <c r="D11" s="304"/>
@@ -13426,23 +13606,23 @@
       <c r="B12" s="297"/>
       <c r="C12" s="298"/>
       <c r="D12" s="296" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="E12" s="293"/>
       <c r="F12" s="292" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="G12" s="293"/>
       <c r="H12" s="292" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="I12" s="293"/>
       <c r="J12" s="292" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="K12" s="293"/>
       <c r="L12" s="292" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="M12" s="293"/>
       <c r="N12" s="2"/>
@@ -13455,7 +13635,7 @@
       <c r="B13" s="299"/>
       <c r="C13" s="300"/>
       <c r="D13" s="188" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E13" s="294"/>
       <c r="F13" s="289"/>
@@ -13473,27 +13653,27 @@
     <row r="14" spans="1:18" customHeight="1" ht="15">
       <c r="A14" s="13"/>
       <c r="B14" s="295" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C14" s="188"/>
       <c r="D14" s="188" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E14" s="294"/>
       <c r="F14" s="290" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="G14" s="291"/>
       <c r="H14" s="290" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="I14" s="291"/>
       <c r="J14" s="290" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="K14" s="291"/>
       <c r="L14" s="290" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="M14" s="291"/>
       <c r="N14" s="2"/>
@@ -13502,9 +13682,13 @@
     </row>
     <row r="15" spans="1:18" customHeight="1" ht="15">
       <c r="A15" s="13"/>
-      <c r="B15" s="301"/>
+      <c r="B15" s="301" t="s">
+        <v>117</v>
+      </c>
       <c r="C15" s="302"/>
-      <c r="D15" s="286"/>
+      <c r="D15" s="286" t="s">
+        <v>144</v>
+      </c>
       <c r="E15" s="287"/>
       <c r="F15" s="301"/>
       <c r="G15" s="302"/>
@@ -13520,9 +13704,13 @@
     </row>
     <row r="16" spans="1:18" customHeight="1" ht="15">
       <c r="A16" s="13"/>
-      <c r="B16" s="285"/>
+      <c r="B16" s="285" t="s">
+        <v>100</v>
+      </c>
       <c r="C16" s="286"/>
-      <c r="D16" s="286"/>
+      <c r="D16" s="286" t="s">
+        <v>145</v>
+      </c>
       <c r="E16" s="287"/>
       <c r="F16" s="285"/>
       <c r="G16" s="286"/>
@@ -14128,7 +14316,7 @@
       <c r="B2" s="11"/>
       <c r="C2" s="4"/>
       <c r="D2" s="252" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="E2" s="252"/>
       <c r="F2" s="252"/>
@@ -14138,7 +14326,7 @@
       <c r="J2" s="252"/>
       <c r="K2" s="252"/>
       <c r="L2" s="253" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="M2" s="253"/>
       <c r="N2" s="10"/>
@@ -14178,14 +14366,14 @@
     <row r="5" spans="1:16" customHeight="1" ht="15" s="31" customFormat="1">
       <c r="A5" s="5"/>
       <c r="B5" s="235" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C5" s="236"/>
       <c r="D5" s="236"/>
       <c r="E5" s="236"/>
       <c r="F5" s="237"/>
       <c r="G5" s="235" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="H5" s="236"/>
       <c r="I5" s="236"/>
@@ -14299,11 +14487,11 @@
       <c r="A11" s="13"/>
       <c r="B11" s="246"/>
       <c r="C11" s="329" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="D11" s="330"/>
       <c r="E11" s="330">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="234"/>
       <c r="G11" s="234"/>
@@ -14441,7 +14629,7 @@
       <c r="H18" s="234"/>
       <c r="I18" s="308"/>
       <c r="J18" s="312" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="K18" s="312"/>
       <c r="L18" s="312"/>
@@ -14655,7 +14843,7 @@
     <row r="30" spans="1:16" customHeight="1" ht="15">
       <c r="A30" s="13"/>
       <c r="B30" s="230" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="C30" s="231"/>
       <c r="D30" s="231"/>
@@ -14674,7 +14862,7 @@
     <row r="31" spans="1:16" customHeight="1" ht="15">
       <c r="A31" s="13"/>
       <c r="B31" s="158" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="C31" s="159"/>
       <c r="D31" s="159"/>
@@ -14685,11 +14873,13 @@
       </c>
       <c r="H31" s="204"/>
       <c r="I31" s="158" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="J31" s="159"/>
       <c r="K31" s="159"/>
-      <c r="L31" s="268"/>
+      <c r="L31" s="268" t="s">
+        <v>153</v>
+      </c>
       <c r="M31" s="269"/>
       <c r="N31" s="2"/>
       <c r="O31" s="31"/>
@@ -15003,7 +15193,7 @@
     <row r="50" spans="1:16" customHeight="1" ht="15">
       <c r="A50" s="13"/>
       <c r="B50" s="191" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="C50" s="192"/>
       <c r="D50" s="192"/>
@@ -15022,7 +15212,7 @@
     <row r="51" spans="1:16" customHeight="1" ht="15">
       <c r="A51" s="13"/>
       <c r="B51" s="25" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="C51" s="26"/>
       <c r="D51" s="27"/>
@@ -15479,7 +15669,7 @@
       <c r="A1" s="331"/>
       <c r="B1" s="332"/>
       <c r="C1" s="332" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="D1" s="332"/>
       <c r="E1" s="332"/>
@@ -15490,17 +15680,17 @@
     </row>
     <row r="2" spans="1:10" customHeight="1" ht="24">
       <c r="A2" s="334" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="B2" s="335"/>
       <c r="C2" s="336"/>
       <c r="D2" s="337">
-        <v>4256137</v>
+        <v>542361</v>
       </c>
       <c r="E2" s="338"/>
       <c r="F2" s="338"/>
       <c r="G2" s="339" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="H2" s="340"/>
       <c r="I2" s="341"/>
@@ -15508,7 +15698,7 @@
     </row>
     <row r="3" spans="1:10" customHeight="1" ht="24">
       <c r="A3" s="348" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="B3" s="349"/>
       <c r="C3" s="350"/>
@@ -15524,7 +15714,7 @@
     </row>
     <row r="4" spans="1:10" customHeight="1" ht="24">
       <c r="A4" s="348" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="B4" s="349"/>
       <c r="C4" s="350"/>
@@ -15550,12 +15740,12 @@
     </row>
     <row r="6" spans="1:10" customHeight="1" ht="24">
       <c r="A6" s="357" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="B6" s="358"/>
       <c r="C6" s="359"/>
       <c r="D6" s="360">
-        <v>8563214</v>
+        <v>856491</v>
       </c>
       <c r="E6" s="361"/>
       <c r="F6" s="361"/>
@@ -15565,11 +15755,13 @@
     </row>
     <row r="7" spans="1:10" customHeight="1" ht="24">
       <c r="A7" s="357" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B7" s="358"/>
       <c r="C7" s="359"/>
-      <c r="D7" s="360"/>
+      <c r="D7" s="360" t="s">
+        <v>163</v>
+      </c>
       <c r="E7" s="361"/>
       <c r="F7" s="361"/>
       <c r="G7" s="342"/>
@@ -15578,11 +15770,13 @@
     </row>
     <row r="8" spans="1:10" customHeight="1" ht="24">
       <c r="A8" s="362" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="B8" s="363"/>
       <c r="C8" s="364"/>
-      <c r="D8" s="365"/>
+      <c r="D8" s="365" t="s">
+        <v>165</v>
+      </c>
       <c r="E8" s="366"/>
       <c r="F8" s="366"/>
       <c r="G8" s="345"/>
@@ -15604,7 +15798,7 @@
       <c r="A10" s="331"/>
       <c r="B10" s="332"/>
       <c r="C10" s="332" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="D10" s="332"/>
       <c r="E10" s="332"/>
@@ -15615,24 +15809,24 @@
     </row>
     <row r="11" spans="1:10" customHeight="1" ht="24">
       <c r="A11" s="334" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="B11" s="335"/>
       <c r="C11" s="336"/>
       <c r="D11" s="337">
-        <v>4256137</v>
+        <v>542361</v>
       </c>
       <c r="E11" s="338"/>
       <c r="F11" s="338"/>
       <c r="G11" s="339" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="H11" s="340"/>
       <c r="I11" s="341"/>
     </row>
     <row r="12" spans="1:10" customHeight="1" ht="24">
       <c r="A12" s="348" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="B12" s="349"/>
       <c r="C12" s="350"/>
@@ -15647,7 +15841,7 @@
     </row>
     <row r="13" spans="1:10" customHeight="1" ht="24">
       <c r="A13" s="348" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="B13" s="349"/>
       <c r="C13" s="350"/>
@@ -15673,12 +15867,12 @@
     </row>
     <row r="15" spans="1:10" customHeight="1" ht="24">
       <c r="A15" s="357" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="B15" s="358"/>
       <c r="C15" s="359"/>
       <c r="D15" s="360">
-        <v>8563214</v>
+        <v>856491</v>
       </c>
       <c r="E15" s="361"/>
       <c r="F15" s="361"/>
@@ -15688,11 +15882,13 @@
     </row>
     <row r="16" spans="1:10" customHeight="1" ht="24">
       <c r="A16" s="357" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B16" s="358"/>
       <c r="C16" s="359"/>
-      <c r="D16" s="360"/>
+      <c r="D16" s="360" t="s">
+        <v>163</v>
+      </c>
       <c r="E16" s="361"/>
       <c r="F16" s="361"/>
       <c r="G16" s="342"/>
@@ -15701,11 +15897,13 @@
     </row>
     <row r="17" spans="1:10" customHeight="1" ht="24">
       <c r="A17" s="362" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="B17" s="363"/>
       <c r="C17" s="364"/>
-      <c r="D17" s="365"/>
+      <c r="D17" s="365" t="s">
+        <v>165</v>
+      </c>
       <c r="E17" s="366"/>
       <c r="F17" s="366"/>
       <c r="G17" s="345"/>
@@ -15727,7 +15925,7 @@
       <c r="A19" s="331"/>
       <c r="B19" s="332"/>
       <c r="C19" s="332" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="D19" s="332"/>
       <c r="E19" s="332"/>
@@ -15738,24 +15936,24 @@
     </row>
     <row r="20" spans="1:10" customHeight="1" ht="24">
       <c r="A20" s="334" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="B20" s="335"/>
       <c r="C20" s="336"/>
       <c r="D20" s="337">
-        <v>4256137</v>
+        <v>542361</v>
       </c>
       <c r="E20" s="338"/>
       <c r="F20" s="338"/>
       <c r="G20" s="339" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="H20" s="340"/>
       <c r="I20" s="341"/>
     </row>
     <row r="21" spans="1:10" customHeight="1" ht="24">
       <c r="A21" s="348" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="B21" s="349"/>
       <c r="C21" s="350"/>
@@ -15770,7 +15968,7 @@
     </row>
     <row r="22" spans="1:10" customHeight="1" ht="24">
       <c r="A22" s="348" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="B22" s="349"/>
       <c r="C22" s="350"/>
@@ -15796,12 +15994,12 @@
     </row>
     <row r="24" spans="1:10" customHeight="1" ht="24">
       <c r="A24" s="357" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="B24" s="358"/>
       <c r="C24" s="359"/>
       <c r="D24" s="360">
-        <v>8563214</v>
+        <v>856491</v>
       </c>
       <c r="E24" s="361"/>
       <c r="F24" s="361"/>
@@ -15811,11 +16009,13 @@
     </row>
     <row r="25" spans="1:10" customHeight="1" ht="24">
       <c r="A25" s="357" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B25" s="358"/>
       <c r="C25" s="359"/>
-      <c r="D25" s="360"/>
+      <c r="D25" s="360" t="s">
+        <v>163</v>
+      </c>
       <c r="E25" s="361"/>
       <c r="F25" s="361"/>
       <c r="G25" s="342"/>
@@ -15824,11 +16024,13 @@
     </row>
     <row r="26" spans="1:10" customHeight="1" ht="24">
       <c r="A26" s="362" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="B26" s="363"/>
       <c r="C26" s="364"/>
-      <c r="D26" s="365"/>
+      <c r="D26" s="365" t="s">
+        <v>165</v>
+      </c>
       <c r="E26" s="366"/>
       <c r="F26" s="366"/>
       <c r="G26" s="345"/>
@@ -15850,7 +16052,7 @@
       <c r="A28" s="370"/>
       <c r="B28" s="371"/>
       <c r="C28" s="371" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="D28" s="371"/>
       <c r="E28" s="371"/>
@@ -15861,24 +16063,24 @@
     </row>
     <row r="29" spans="1:10" customHeight="1" ht="24">
       <c r="A29" s="334" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="B29" s="335"/>
       <c r="C29" s="336"/>
       <c r="D29" s="337">
-        <v>4256137</v>
+        <v>542361</v>
       </c>
       <c r="E29" s="338"/>
       <c r="F29" s="338"/>
       <c r="G29" s="339" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="H29" s="340"/>
       <c r="I29" s="341"/>
     </row>
     <row r="30" spans="1:10" customHeight="1" ht="24">
       <c r="A30" s="348" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="B30" s="349"/>
       <c r="C30" s="350"/>
@@ -15893,7 +16095,7 @@
     </row>
     <row r="31" spans="1:10" customHeight="1" ht="24">
       <c r="A31" s="348" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="B31" s="349"/>
       <c r="C31" s="350"/>
@@ -15919,12 +16121,12 @@
     </row>
     <row r="33" spans="1:10" customHeight="1" ht="24">
       <c r="A33" s="357" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="B33" s="358"/>
       <c r="C33" s="359"/>
       <c r="D33" s="360">
-        <v>8563214</v>
+        <v>856491</v>
       </c>
       <c r="E33" s="361"/>
       <c r="F33" s="361"/>
@@ -15934,11 +16136,13 @@
     </row>
     <row r="34" spans="1:10" customHeight="1" ht="24">
       <c r="A34" s="357" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B34" s="358"/>
       <c r="C34" s="359"/>
-      <c r="D34" s="360"/>
+      <c r="D34" s="360" t="s">
+        <v>163</v>
+      </c>
       <c r="E34" s="361"/>
       <c r="F34" s="361"/>
       <c r="G34" s="342"/>
@@ -15947,11 +16151,13 @@
     </row>
     <row r="35" spans="1:10" customHeight="1" ht="24">
       <c r="A35" s="362" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="B35" s="363"/>
       <c r="C35" s="364"/>
-      <c r="D35" s="365"/>
+      <c r="D35" s="365" t="s">
+        <v>165</v>
+      </c>
       <c r="E35" s="366"/>
       <c r="F35" s="366"/>
       <c r="G35" s="345"/>
@@ -16099,7 +16305,7 @@
       <c r="B2" s="11"/>
       <c r="C2" s="4"/>
       <c r="D2" s="252" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="E2" s="252"/>
       <c r="F2" s="252"/>
@@ -16109,7 +16315,7 @@
       <c r="J2" s="252"/>
       <c r="K2" s="252"/>
       <c r="L2" s="253" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="M2" s="253"/>
       <c r="N2" s="10"/>
@@ -16149,21 +16355,21 @@
     <row r="5" spans="1:18" customHeight="1" ht="15">
       <c r="A5" s="10"/>
       <c r="B5" s="235" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C5" s="236"/>
       <c r="D5" s="236"/>
       <c r="E5" s="236"/>
       <c r="F5" s="237"/>
       <c r="G5" s="235" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="H5" s="236"/>
       <c r="I5" s="236"/>
       <c r="J5" s="236"/>
       <c r="K5" s="237"/>
       <c r="L5" s="235" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="M5" s="237"/>
       <c r="N5" s="10"/>
@@ -16178,14 +16384,14 @@
       <c r="E6" s="248"/>
       <c r="F6" s="249"/>
       <c r="G6" s="247">
-        <v>8563214</v>
+        <v>856491</v>
       </c>
       <c r="H6" s="248"/>
       <c r="I6" s="248"/>
       <c r="J6" s="248"/>
       <c r="K6" s="249"/>
       <c r="L6" s="306" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="M6" s="251"/>
       <c r="N6" s="10"/>
@@ -16210,7 +16416,7 @@
     <row r="8" spans="1:18" customHeight="1" ht="15">
       <c r="A8" s="13"/>
       <c r="B8" s="230" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C8" s="231"/>
       <c r="D8" s="231"/>
@@ -16231,7 +16437,7 @@
     <row r="9" spans="1:18" customHeight="1" ht="15">
       <c r="A9" s="13"/>
       <c r="B9" s="383" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C9" s="222"/>
       <c r="D9" s="222"/>
@@ -16405,7 +16611,7 @@
     <row r="18" spans="1:18" customHeight="1" ht="15">
       <c r="A18" s="13"/>
       <c r="B18" s="383" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="C18" s="222"/>
       <c r="D18" s="222"/>
@@ -16502,7 +16708,7 @@
     <row r="23" spans="1:18" customHeight="1" ht="15">
       <c r="A23" s="13"/>
       <c r="B23" s="165" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="C23" s="166"/>
       <c r="D23" s="166"/>
@@ -16523,25 +16729,25 @@
     <row r="24" spans="1:18" customHeight="1" ht="15">
       <c r="A24" s="13"/>
       <c r="B24" s="176" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="C24" s="176"/>
       <c r="D24" s="176"/>
       <c r="E24" s="176"/>
       <c r="F24" s="176" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="G24" s="176"/>
       <c r="H24" s="176" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="I24" s="176"/>
       <c r="J24" s="176" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="K24" s="176"/>
       <c r="L24" s="176" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="M24" s="176"/>
       <c r="N24" s="3"/>
@@ -16752,7 +16958,7 @@
     <row r="35" spans="1:18" customHeight="1" ht="15">
       <c r="A35" s="13"/>
       <c r="B35" s="230" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="C35" s="231"/>
       <c r="D35" s="231"/>
@@ -16768,7 +16974,7 @@
       <c r="N35" s="2"/>
       <c r="O35" s="31"/>
       <c r="P35" s="49" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="Q35" s="29"/>
       <c r="R35" s="31"/>
@@ -16790,7 +16996,7 @@
       <c r="N36" s="2"/>
       <c r="O36" s="31"/>
       <c r="P36" s="48" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="Q36" s="29"/>
       <c r="R36" s="31"/>
@@ -16812,7 +17018,7 @@
       <c r="N37" s="2"/>
       <c r="O37" s="31"/>
       <c r="P37" s="48" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="Q37" s="29"/>
       <c r="R37" s="31"/>
@@ -16834,7 +17040,7 @@
       <c r="N38" s="2"/>
       <c r="O38" s="31"/>
       <c r="P38" s="48" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="Q38" s="29"/>
       <c r="R38" s="31"/>
@@ -16856,7 +17062,7 @@
       <c r="N39" s="3"/>
       <c r="O39" s="30"/>
       <c r="P39" s="48" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="Q39" s="29"/>
       <c r="R39" s="30"/>
@@ -16877,7 +17083,7 @@
       <c r="M40" s="266"/>
       <c r="N40" s="10"/>
       <c r="P40" s="48" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -18090,7 +18296,7 @@
       <c r="N2" s="391"/>
       <c r="O2" s="392"/>
       <c r="P2" s="389" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="Q2" s="389"/>
       <c r="R2" s="389"/>
@@ -18149,7 +18355,7 @@
       <c r="BS2" s="389"/>
       <c r="BT2" s="389"/>
       <c r="BU2" s="413" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="BV2" s="414"/>
       <c r="BW2" s="414"/>
@@ -18338,7 +18544,7 @@
     <row r="5" spans="1:86" customHeight="1" ht="24">
       <c r="A5" s="88"/>
       <c r="B5" s="397" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C5" s="398"/>
       <c r="D5" s="398"/>
@@ -18371,7 +18577,7 @@
       <c r="AE5" s="398"/>
       <c r="AF5" s="399"/>
       <c r="AG5" s="397" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="AH5" s="398"/>
       <c r="AI5" s="398"/>
@@ -18413,7 +18619,7 @@
       <c r="BS5" s="398"/>
       <c r="BT5" s="399"/>
       <c r="BU5" s="398" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="BV5" s="398"/>
       <c r="BW5" s="398"/>
@@ -18463,7 +18669,7 @@
       <c r="AE6" s="387"/>
       <c r="AF6" s="388"/>
       <c r="AG6" s="386">
-        <v>8563214</v>
+        <v>856491</v>
       </c>
       <c r="AH6" s="387"/>
       <c r="AI6" s="387"/>
@@ -18505,7 +18711,7 @@
       <c r="BS6" s="387"/>
       <c r="BT6" s="388"/>
       <c r="BU6" s="387" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="BV6" s="387"/>
       <c r="BW6" s="387"/>
@@ -18608,7 +18814,7 @@
     <row r="8" spans="1:86" customHeight="1" ht="24">
       <c r="A8" s="88"/>
       <c r="B8" s="395" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="C8" s="395"/>
       <c r="D8" s="395"/>
@@ -18693,14 +18899,14 @@
       <c r="CE8" s="395"/>
       <c r="CF8" s="88"/>
       <c r="CH8" s="49" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:86" customHeight="1" ht="24">
       <c r="A9" s="88"/>
       <c r="B9" s="54"/>
       <c r="C9" s="406" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="D9" s="406"/>
       <c r="E9" s="406"/>
@@ -18719,7 +18925,7 @@
       <c r="R9" s="55"/>
       <c r="S9" s="55"/>
       <c r="T9" s="406" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="U9" s="406"/>
       <c r="V9" s="406"/>
@@ -18737,7 +18943,7 @@
       <c r="AH9" s="55"/>
       <c r="AI9" s="55"/>
       <c r="AJ9" s="406" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="AK9" s="406"/>
       <c r="AL9" s="406"/>
@@ -18757,7 +18963,7 @@
       <c r="AZ9" s="55"/>
       <c r="BA9" s="55"/>
       <c r="BB9" s="406" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="BC9" s="406"/>
       <c r="BD9" s="406"/>
@@ -18790,7 +18996,7 @@
       <c r="CE9" s="56"/>
       <c r="CF9" s="88"/>
       <c r="CH9" s="157" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:86" customHeight="1" ht="24">
@@ -18801,7 +19007,7 @@
       <c r="E10" s="60"/>
       <c r="F10" s="61"/>
       <c r="G10" s="62" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="H10" s="407"/>
       <c r="I10" s="408"/>
@@ -18820,7 +19026,7 @@
       <c r="V10" s="58"/>
       <c r="W10" s="61"/>
       <c r="X10" s="62" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="Y10" s="407"/>
       <c r="Z10" s="408"/>
@@ -18839,7 +19045,7 @@
       <c r="AM10" s="63"/>
       <c r="AN10" s="63"/>
       <c r="AO10" s="62" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="AP10" s="400"/>
       <c r="AQ10" s="401"/>
@@ -18858,7 +19064,7 @@
       <c r="BD10" s="60"/>
       <c r="BE10" s="61"/>
       <c r="BF10" s="62" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="BG10" s="407"/>
       <c r="BH10" s="408"/>
@@ -18887,7 +19093,7 @@
       <c r="CE10" s="64"/>
       <c r="CF10" s="88"/>
       <c r="CH10" s="48" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:86" customHeight="1" ht="24">
@@ -18976,7 +19182,7 @@
       <c r="CE11" s="64"/>
       <c r="CF11" s="88"/>
       <c r="CH11" s="48" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:86" customHeight="1" ht="24">
@@ -18989,7 +19195,7 @@
       <c r="G12" s="61"/>
       <c r="H12" s="61"/>
       <c r="I12" s="62" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="J12" s="400"/>
       <c r="K12" s="401"/>
@@ -19008,7 +19214,7 @@
       <c r="X12" s="58"/>
       <c r="Y12" s="61"/>
       <c r="Z12" s="62" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="AA12" s="400"/>
       <c r="AB12" s="401"/>
@@ -19027,7 +19233,7 @@
       <c r="AO12" s="63"/>
       <c r="AP12" s="63"/>
       <c r="AQ12" s="62" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="AR12" s="400"/>
       <c r="AS12" s="401"/>
@@ -19046,7 +19252,7 @@
       <c r="BF12" s="61"/>
       <c r="BG12" s="61"/>
       <c r="BH12" s="62" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="BI12" s="407"/>
       <c r="BJ12" s="408"/>
@@ -19073,7 +19279,7 @@
       <c r="CE12" s="64"/>
       <c r="CF12" s="88"/>
       <c r="CH12" s="136" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:86" customHeight="1" ht="24">
@@ -19175,7 +19381,7 @@
       <c r="I14" s="61"/>
       <c r="J14" s="61"/>
       <c r="K14" s="62" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="L14" s="400"/>
       <c r="M14" s="401"/>
@@ -19194,7 +19400,7 @@
       <c r="Z14" s="58"/>
       <c r="AA14" s="61"/>
       <c r="AB14" s="62" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="AC14" s="400"/>
       <c r="AD14" s="401"/>
@@ -19213,7 +19419,7 @@
       <c r="AQ14" s="63"/>
       <c r="AR14" s="63"/>
       <c r="AS14" s="62" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="AT14" s="400"/>
       <c r="AU14" s="401"/>
@@ -19232,7 +19438,7 @@
       <c r="BH14" s="61"/>
       <c r="BI14" s="61"/>
       <c r="BJ14" s="62" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="BK14" s="400"/>
       <c r="BL14" s="401"/>
@@ -19357,7 +19563,7 @@
       <c r="K16" s="61"/>
       <c r="L16" s="61"/>
       <c r="M16" s="62" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="N16" s="400"/>
       <c r="O16" s="401"/>
@@ -19376,7 +19582,7 @@
       <c r="AB16" s="58"/>
       <c r="AC16" s="61"/>
       <c r="AD16" s="62" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="AE16" s="400"/>
       <c r="AF16" s="401"/>
@@ -19395,7 +19601,7 @@
       <c r="AS16" s="63"/>
       <c r="AT16" s="63"/>
       <c r="AU16" s="62" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="AV16" s="400"/>
       <c r="AW16" s="401"/>
@@ -19414,7 +19620,7 @@
       <c r="BJ16" s="61"/>
       <c r="BK16" s="61"/>
       <c r="BL16" s="62" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="BM16" s="400"/>
       <c r="BN16" s="401"/>
@@ -19539,7 +19745,7 @@
       <c r="M18" s="61"/>
       <c r="N18" s="61"/>
       <c r="O18" s="62" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="P18" s="400"/>
       <c r="Q18" s="401"/>
@@ -19558,7 +19764,7 @@
       <c r="AD18" s="58"/>
       <c r="AE18" s="61"/>
       <c r="AF18" s="62" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="AG18" s="400"/>
       <c r="AH18" s="401"/>
@@ -19577,7 +19783,7 @@
       <c r="AU18" s="63"/>
       <c r="AV18" s="63"/>
       <c r="AW18" s="62" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="AX18" s="400"/>
       <c r="AY18" s="401"/>
@@ -19596,7 +19802,7 @@
       <c r="BL18" s="61"/>
       <c r="BM18" s="61"/>
       <c r="BN18" s="62" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="BO18" s="400"/>
       <c r="BP18" s="401"/>
@@ -19721,7 +19927,7 @@
       <c r="O20" s="61"/>
       <c r="P20" s="61"/>
       <c r="Q20" s="62" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="R20" s="400"/>
       <c r="S20" s="401"/>
@@ -19740,7 +19946,7 @@
       <c r="AF20" s="58"/>
       <c r="AG20" s="61"/>
       <c r="AH20" s="62" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="AI20" s="400"/>
       <c r="AJ20" s="401"/>
@@ -19759,7 +19965,7 @@
       <c r="AW20" s="63"/>
       <c r="AX20" s="63"/>
       <c r="AY20" s="62" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="AZ20" s="400"/>
       <c r="BA20" s="401"/>
@@ -19778,7 +19984,7 @@
       <c r="BN20" s="61"/>
       <c r="BO20" s="61"/>
       <c r="BP20" s="62" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="BQ20" s="400"/>
       <c r="BR20" s="401"/>
@@ -19988,7 +20194,7 @@
       <c r="P23" s="59"/>
       <c r="Q23" s="59"/>
       <c r="R23" s="62" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="S23" s="400"/>
       <c r="T23" s="401"/>
@@ -20007,7 +20213,7 @@
       <c r="AG23" s="58"/>
       <c r="AH23" s="58"/>
       <c r="AI23" s="62" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="AJ23" s="400"/>
       <c r="AK23" s="401"/>
@@ -20026,7 +20232,7 @@
       <c r="AX23" s="63"/>
       <c r="AY23" s="63"/>
       <c r="AZ23" s="62" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="BA23" s="400"/>
       <c r="BB23" s="401"/>
@@ -20045,7 +20251,7 @@
       <c r="BO23" s="60"/>
       <c r="BP23" s="60"/>
       <c r="BQ23" s="62" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="BR23" s="400"/>
       <c r="BS23" s="401"/>
@@ -20166,7 +20372,7 @@
       <c r="N25" s="59"/>
       <c r="O25" s="59"/>
       <c r="P25" s="62" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="Q25" s="400"/>
       <c r="R25" s="401"/>
@@ -20185,7 +20391,7 @@
       <c r="AE25" s="58"/>
       <c r="AF25" s="58"/>
       <c r="AG25" s="62" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="AH25" s="400"/>
       <c r="AI25" s="401"/>
@@ -20204,7 +20410,7 @@
       <c r="AV25" s="63"/>
       <c r="AW25" s="63"/>
       <c r="AX25" s="62" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="AY25" s="400"/>
       <c r="AZ25" s="401"/>
@@ -20223,7 +20429,7 @@
       <c r="BM25" s="60"/>
       <c r="BN25" s="60"/>
       <c r="BO25" s="62" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="BP25" s="400"/>
       <c r="BQ25" s="401"/>
@@ -20344,7 +20550,7 @@
       <c r="L27" s="58"/>
       <c r="M27" s="59"/>
       <c r="N27" s="62" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="O27" s="400"/>
       <c r="P27" s="401"/>
@@ -20363,7 +20569,7 @@
       <c r="AC27" s="58"/>
       <c r="AD27" s="58"/>
       <c r="AE27" s="62" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="AF27" s="400"/>
       <c r="AG27" s="401"/>
@@ -20382,7 +20588,7 @@
       <c r="AT27" s="63"/>
       <c r="AU27" s="63"/>
       <c r="AV27" s="62" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="AW27" s="400"/>
       <c r="AX27" s="401"/>
@@ -20401,7 +20607,7 @@
       <c r="BK27" s="58"/>
       <c r="BL27" s="60"/>
       <c r="BM27" s="62" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="BN27" s="400"/>
       <c r="BO27" s="401"/>
@@ -20522,7 +20728,7 @@
       <c r="J29" s="58"/>
       <c r="K29" s="58"/>
       <c r="L29" s="62" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="M29" s="400"/>
       <c r="N29" s="401"/>
@@ -20541,7 +20747,7 @@
       <c r="AA29" s="58"/>
       <c r="AB29" s="58"/>
       <c r="AC29" s="62" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="AD29" s="400"/>
       <c r="AE29" s="401"/>
@@ -20560,7 +20766,7 @@
       <c r="AR29" s="63"/>
       <c r="AS29" s="63"/>
       <c r="AT29" s="62" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="AU29" s="400"/>
       <c r="AV29" s="401"/>
@@ -20579,7 +20785,7 @@
       <c r="BI29" s="58"/>
       <c r="BJ29" s="60"/>
       <c r="BK29" s="62" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="BL29" s="400"/>
       <c r="BM29" s="401"/>
@@ -20700,7 +20906,7 @@
       <c r="H31" s="58"/>
       <c r="I31" s="58"/>
       <c r="J31" s="62" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="K31" s="400"/>
       <c r="L31" s="401"/>
@@ -20719,7 +20925,7 @@
       <c r="Y31" s="58"/>
       <c r="Z31" s="58"/>
       <c r="AA31" s="62" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="AB31" s="400"/>
       <c r="AC31" s="401"/>
@@ -20738,7 +20944,7 @@
       <c r="AP31" s="63"/>
       <c r="AQ31" s="63"/>
       <c r="AR31" s="62" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="AS31" s="400"/>
       <c r="AT31" s="401"/>
@@ -20757,7 +20963,7 @@
       <c r="BG31" s="58"/>
       <c r="BH31" s="60"/>
       <c r="BI31" s="62" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="BJ31" s="400"/>
       <c r="BK31" s="401"/>
@@ -20878,7 +21084,7 @@
       <c r="F33" s="58"/>
       <c r="G33" s="58"/>
       <c r="H33" s="62" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="I33" s="400"/>
       <c r="J33" s="401"/>
@@ -20897,7 +21103,7 @@
       <c r="W33" s="58"/>
       <c r="X33" s="58"/>
       <c r="Y33" s="62" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="Z33" s="400"/>
       <c r="AA33" s="401"/>
@@ -20916,7 +21122,7 @@
       <c r="AN33" s="63"/>
       <c r="AO33" s="63"/>
       <c r="AP33" s="62" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="AQ33" s="400"/>
       <c r="AR33" s="401"/>
@@ -20935,7 +21141,7 @@
       <c r="BE33" s="58"/>
       <c r="BF33" s="60"/>
       <c r="BG33" s="62" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="BH33" s="400"/>
       <c r="BI33" s="401"/>
@@ -21053,7 +21259,7 @@
       <c r="A35" s="88"/>
       <c r="B35" s="75"/>
       <c r="C35" s="418" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="D35" s="418"/>
       <c r="E35" s="418"/>
@@ -21072,7 +21278,7 @@
       <c r="R35" s="76"/>
       <c r="S35" s="76"/>
       <c r="T35" s="418" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="U35" s="418"/>
       <c r="V35" s="418"/>
@@ -21091,7 +21297,7 @@
       <c r="AI35" s="76"/>
       <c r="AJ35" s="76"/>
       <c r="AK35" s="418" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="AL35" s="418"/>
       <c r="AM35" s="418"/>
@@ -21111,7 +21317,7 @@
       <c r="BA35" s="76"/>
       <c r="BB35" s="76"/>
       <c r="BC35" s="418" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="BD35" s="418"/>
       <c r="BE35" s="418"/>
@@ -21232,7 +21438,7 @@
     <row r="37" spans="1:86" customHeight="1" ht="24">
       <c r="A37" s="88"/>
       <c r="B37" s="396" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="C37" s="396"/>
       <c r="D37" s="396"/>
@@ -21406,7 +21612,7 @@
     <row r="39" spans="1:86" customHeight="1" ht="24">
       <c r="A39" s="88"/>
       <c r="B39" s="417" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="C39" s="417"/>
       <c r="D39" s="417"/>
@@ -21494,7 +21700,7 @@
     <row r="40" spans="1:86" customHeight="1" ht="24">
       <c r="A40" s="88"/>
       <c r="B40" s="416" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C40" s="416"/>
       <c r="D40" s="416"/>
@@ -21537,7 +21743,7 @@
       <c r="AO40" s="416"/>
       <c r="AP40" s="416"/>
       <c r="AQ40" s="416" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="AR40" s="416"/>
       <c r="AS40" s="416"/>
@@ -21584,7 +21790,7 @@
     <row r="41" spans="1:86" customHeight="1" ht="25">
       <c r="A41" s="88"/>
       <c r="B41" s="416" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="C41" s="416"/>
       <c r="D41" s="416"/>
@@ -21627,7 +21833,7 @@
       <c r="AO41" s="416"/>
       <c r="AP41" s="416"/>
       <c r="AQ41" s="416" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AR41" s="416"/>
       <c r="AS41" s="416"/>
@@ -21674,7 +21880,7 @@
     <row r="42" spans="1:86" customHeight="1" ht="25">
       <c r="A42" s="88"/>
       <c r="B42" s="419" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="C42" s="416"/>
       <c r="D42" s="416"/>
@@ -21848,12 +22054,12 @@
     <row r="44" spans="1:86" customHeight="1" ht="25">
       <c r="A44" s="88"/>
       <c r="B44" s="428" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="C44" s="425"/>
       <c r="D44" s="425"/>
       <c r="E44" s="425" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="F44" s="425"/>
       <c r="G44" s="425"/>
@@ -21864,7 +22070,7 @@
       <c r="L44" s="425"/>
       <c r="M44" s="425"/>
       <c r="N44" s="425" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="O44" s="425"/>
       <c r="P44" s="425"/>
@@ -21887,7 +22093,7 @@
       <c r="AG44" s="425"/>
       <c r="AH44" s="425"/>
       <c r="AI44" s="425" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="AJ44" s="425"/>
       <c r="AK44" s="425"/>
@@ -21897,7 +22103,7 @@
       <c r="AO44" s="425"/>
       <c r="AP44" s="425"/>
       <c r="AQ44" s="425" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="AR44" s="425"/>
       <c r="AS44" s="425"/>
@@ -21949,7 +22155,7 @@
       <c r="C45" s="421"/>
       <c r="D45" s="421"/>
       <c r="E45" s="421" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="F45" s="421"/>
       <c r="G45" s="421"/>
@@ -22042,7 +22248,7 @@
       <c r="C46" s="421"/>
       <c r="D46" s="421"/>
       <c r="E46" s="421" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="F46" s="421"/>
       <c r="G46" s="421"/>
@@ -22135,7 +22341,7 @@
       <c r="C47" s="421"/>
       <c r="D47" s="421"/>
       <c r="E47" s="421" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="F47" s="421"/>
       <c r="G47" s="421"/>
@@ -22228,7 +22434,7 @@
       <c r="C48" s="421"/>
       <c r="D48" s="421"/>
       <c r="E48" s="421" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="F48" s="421"/>
       <c r="G48" s="421"/>
@@ -22321,7 +22527,7 @@
       <c r="C49" s="421"/>
       <c r="D49" s="421"/>
       <c r="E49" s="421" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="F49" s="421"/>
       <c r="G49" s="421"/>
@@ -22414,7 +22620,7 @@
       <c r="C50" s="421"/>
       <c r="D50" s="421"/>
       <c r="E50" s="421" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="F50" s="421"/>
       <c r="G50" s="421"/>
@@ -22507,7 +22713,7 @@
       <c r="C51" s="421"/>
       <c r="D51" s="421"/>
       <c r="E51" s="421" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="F51" s="421"/>
       <c r="G51" s="421"/>
@@ -22600,7 +22806,7 @@
       <c r="C52" s="421"/>
       <c r="D52" s="421"/>
       <c r="E52" s="421" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="F52" s="421"/>
       <c r="G52" s="421"/>
@@ -22693,7 +22899,7 @@
       <c r="C53" s="421"/>
       <c r="D53" s="421"/>
       <c r="E53" s="421" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="F53" s="421"/>
       <c r="G53" s="421"/>
@@ -22786,7 +22992,7 @@
       <c r="C54" s="421"/>
       <c r="D54" s="421"/>
       <c r="E54" s="421" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="F54" s="421"/>
       <c r="G54" s="421"/>
@@ -22879,7 +23085,7 @@
       <c r="C55" s="421"/>
       <c r="D55" s="421"/>
       <c r="E55" s="421" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="F55" s="421"/>
       <c r="G55" s="421"/>
@@ -22972,7 +23178,7 @@
       <c r="C56" s="421"/>
       <c r="D56" s="421"/>
       <c r="E56" s="421" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="F56" s="421"/>
       <c r="G56" s="421"/>
@@ -23065,7 +23271,7 @@
       <c r="C57" s="421"/>
       <c r="D57" s="421"/>
       <c r="E57" s="421" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="F57" s="421"/>
       <c r="G57" s="421"/>
@@ -23075,8 +23281,9 @@
       <c r="K57" s="421"/>
       <c r="L57" s="421"/>
       <c r="M57" s="421"/>
-      <c r="N57" s="416" t="s">
-        <v>248</v>
+      <c r="N57" s="416">
+        <f>AP10</f>
+        <v/>
       </c>
       <c r="O57" s="421"/>
       <c r="P57" s="421"/>
@@ -23098,9 +23305,7 @@
       <c r="AF57" s="421"/>
       <c r="AG57" s="421"/>
       <c r="AH57" s="421"/>
-      <c r="AI57" s="422">
-        <v>2</v>
-      </c>
+      <c r="AI57" s="422"/>
       <c r="AJ57" s="422"/>
       <c r="AK57" s="422"/>
       <c r="AL57" s="422"/>
@@ -23159,7 +23364,7 @@
       <c r="C58" s="421"/>
       <c r="D58" s="421"/>
       <c r="E58" s="421" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="F58" s="421"/>
       <c r="G58" s="421"/>
@@ -23252,7 +23457,7 @@
       <c r="C59" s="421"/>
       <c r="D59" s="421"/>
       <c r="E59" s="421" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="F59" s="421"/>
       <c r="G59" s="421"/>
@@ -23345,7 +23550,7 @@
       <c r="C60" s="421"/>
       <c r="D60" s="421"/>
       <c r="E60" s="421" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="F60" s="421"/>
       <c r="G60" s="421"/>
@@ -23438,7 +23643,7 @@
       <c r="C61" s="421"/>
       <c r="D61" s="421"/>
       <c r="E61" s="421" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="F61" s="421"/>
       <c r="G61" s="421"/>
@@ -23531,7 +23736,7 @@
       <c r="C62" s="421"/>
       <c r="D62" s="421"/>
       <c r="E62" s="421" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="F62" s="421"/>
       <c r="G62" s="421"/>
@@ -23624,7 +23829,7 @@
       <c r="C63" s="421"/>
       <c r="D63" s="421"/>
       <c r="E63" s="421" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="F63" s="421"/>
       <c r="G63" s="421"/>
@@ -23634,8 +23839,9 @@
       <c r="K63" s="421"/>
       <c r="L63" s="421"/>
       <c r="M63" s="421"/>
-      <c r="N63" s="416" t="s">
-        <v>249</v>
+      <c r="N63" s="416">
+        <f>BG10</f>
+        <v/>
       </c>
       <c r="O63" s="421"/>
       <c r="P63" s="421"/>
@@ -23657,9 +23863,7 @@
       <c r="AF63" s="421"/>
       <c r="AG63" s="421"/>
       <c r="AH63" s="421"/>
-      <c r="AI63" s="422">
-        <v>2</v>
-      </c>
+      <c r="AI63" s="422"/>
       <c r="AJ63" s="422"/>
       <c r="AK63" s="422"/>
       <c r="AL63" s="422"/>
@@ -23667,9 +23871,7 @@
       <c r="AN63" s="422"/>
       <c r="AO63" s="422"/>
       <c r="AP63" s="422"/>
-      <c r="AQ63" s="423" t="s">
-        <v>250</v>
-      </c>
+      <c r="AQ63" s="423"/>
       <c r="AR63" s="423"/>
       <c r="AS63" s="423"/>
       <c r="AT63" s="423"/>
@@ -23720,7 +23922,7 @@
       <c r="C64" s="421"/>
       <c r="D64" s="421"/>
       <c r="E64" s="421" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="F64" s="421"/>
       <c r="G64" s="421"/>
@@ -23813,7 +24015,7 @@
       <c r="C65" s="421"/>
       <c r="D65" s="421"/>
       <c r="E65" s="421" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="F65" s="421"/>
       <c r="G65" s="421"/>
@@ -23906,7 +24108,7 @@
       <c r="C66" s="421"/>
       <c r="D66" s="421"/>
       <c r="E66" s="421" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="F66" s="421"/>
       <c r="G66" s="421"/>
@@ -23999,7 +24201,7 @@
       <c r="C67" s="421"/>
       <c r="D67" s="421"/>
       <c r="E67" s="421" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="F67" s="421"/>
       <c r="G67" s="421"/>
@@ -24092,7 +24294,7 @@
       <c r="C68" s="421"/>
       <c r="D68" s="421"/>
       <c r="E68" s="421" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="F68" s="421"/>
       <c r="G68" s="421"/>
@@ -24185,7 +24387,7 @@
       <c r="C69" s="421"/>
       <c r="D69" s="421"/>
       <c r="E69" s="421" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="F69" s="421"/>
       <c r="G69" s="421"/>
@@ -24195,8 +24397,9 @@
       <c r="K69" s="421"/>
       <c r="L69" s="421"/>
       <c r="M69" s="421"/>
-      <c r="N69" s="416" t="s">
-        <v>251</v>
+      <c r="N69" s="416">
+        <f>S23</f>
+        <v/>
       </c>
       <c r="O69" s="421"/>
       <c r="P69" s="421"/>
@@ -24218,9 +24421,7 @@
       <c r="AF69" s="421"/>
       <c r="AG69" s="421"/>
       <c r="AH69" s="421"/>
-      <c r="AI69" s="422">
-        <v>4</v>
-      </c>
+      <c r="AI69" s="422"/>
       <c r="AJ69" s="422"/>
       <c r="AK69" s="422"/>
       <c r="AL69" s="422"/>
@@ -24228,9 +24429,7 @@
       <c r="AN69" s="422"/>
       <c r="AO69" s="422"/>
       <c r="AP69" s="422"/>
-      <c r="AQ69" s="423" t="s">
-        <v>252</v>
-      </c>
+      <c r="AQ69" s="423"/>
       <c r="AR69" s="423"/>
       <c r="AS69" s="423"/>
       <c r="AT69" s="423"/>
@@ -24281,7 +24480,7 @@
       <c r="C70" s="421"/>
       <c r="D70" s="421"/>
       <c r="E70" s="421" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="F70" s="421"/>
       <c r="G70" s="421"/>
@@ -24374,7 +24573,7 @@
       <c r="C71" s="421"/>
       <c r="D71" s="421"/>
       <c r="E71" s="421" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="F71" s="421"/>
       <c r="G71" s="421"/>
@@ -24467,7 +24666,7 @@
       <c r="C72" s="421"/>
       <c r="D72" s="421"/>
       <c r="E72" s="421" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="F72" s="421"/>
       <c r="G72" s="421"/>
@@ -24560,7 +24759,7 @@
       <c r="C73" s="421"/>
       <c r="D73" s="421"/>
       <c r="E73" s="421" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="F73" s="421"/>
       <c r="G73" s="421"/>
@@ -24653,7 +24852,7 @@
       <c r="C74" s="421"/>
       <c r="D74" s="421"/>
       <c r="E74" s="421" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="F74" s="421"/>
       <c r="G74" s="421"/>
@@ -24746,7 +24945,7 @@
       <c r="C75" s="421"/>
       <c r="D75" s="421"/>
       <c r="E75" s="421" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="F75" s="421"/>
       <c r="G75" s="421"/>
@@ -24839,7 +25038,7 @@
       <c r="C76" s="421"/>
       <c r="D76" s="421"/>
       <c r="E76" s="421" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="F76" s="421"/>
       <c r="G76" s="421"/>
@@ -24932,7 +25131,7 @@
       <c r="C77" s="421"/>
       <c r="D77" s="421"/>
       <c r="E77" s="421" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="F77" s="421"/>
       <c r="G77" s="421"/>
@@ -25025,7 +25224,7 @@
       <c r="C78" s="421"/>
       <c r="D78" s="421"/>
       <c r="E78" s="421" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="F78" s="421"/>
       <c r="G78" s="421"/>
@@ -25118,7 +25317,7 @@
       <c r="C79" s="421"/>
       <c r="D79" s="421"/>
       <c r="E79" s="421" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="F79" s="421"/>
       <c r="G79" s="421"/>
@@ -25211,7 +25410,7 @@
       <c r="C80" s="421"/>
       <c r="D80" s="421"/>
       <c r="E80" s="421" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="F80" s="421"/>
       <c r="G80" s="421"/>
@@ -25304,7 +25503,7 @@
       <c r="C81" s="421"/>
       <c r="D81" s="421"/>
       <c r="E81" s="421" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="F81" s="421"/>
       <c r="G81" s="421"/>
@@ -25397,7 +25596,7 @@
       <c r="C82" s="421"/>
       <c r="D82" s="421"/>
       <c r="E82" s="421" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="F82" s="421"/>
       <c r="G82" s="421"/>
@@ -25490,7 +25689,7 @@
       <c r="C83" s="421"/>
       <c r="D83" s="421"/>
       <c r="E83" s="421" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="F83" s="421"/>
       <c r="G83" s="421"/>
@@ -25583,7 +25782,7 @@
       <c r="C84" s="421"/>
       <c r="D84" s="421"/>
       <c r="E84" s="421" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="F84" s="421"/>
       <c r="G84" s="421"/>
@@ -25676,7 +25875,7 @@
       <c r="C85" s="421"/>
       <c r="D85" s="421"/>
       <c r="E85" s="421" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="F85" s="421"/>
       <c r="G85" s="421"/>
@@ -25769,7 +25968,7 @@
       <c r="C86" s="421"/>
       <c r="D86" s="421"/>
       <c r="E86" s="421" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="F86" s="421"/>
       <c r="G86" s="421"/>
@@ -25862,7 +26061,7 @@
       <c r="C87" s="421"/>
       <c r="D87" s="421"/>
       <c r="E87" s="421" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="F87" s="421"/>
       <c r="G87" s="421"/>
@@ -25955,7 +26154,7 @@
       <c r="C88" s="421"/>
       <c r="D88" s="421"/>
       <c r="E88" s="421" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="F88" s="421"/>
       <c r="G88" s="421"/>
@@ -26048,7 +26247,7 @@
       <c r="C89" s="421"/>
       <c r="D89" s="421"/>
       <c r="E89" s="421" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="F89" s="421"/>
       <c r="G89" s="421"/>
@@ -26141,7 +26340,7 @@
       <c r="C90" s="421"/>
       <c r="D90" s="421"/>
       <c r="E90" s="421" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="F90" s="421"/>
       <c r="G90" s="421"/>
@@ -26234,7 +26433,7 @@
       <c r="C91" s="421"/>
       <c r="D91" s="421"/>
       <c r="E91" s="421" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="F91" s="421"/>
       <c r="G91" s="421"/>
@@ -26327,7 +26526,7 @@
       <c r="C92" s="430"/>
       <c r="D92" s="430"/>
       <c r="E92" s="430" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="F92" s="430"/>
       <c r="G92" s="430"/>
@@ -26960,7 +27159,7 @@
       <c r="B2" s="11"/>
       <c r="C2" s="4"/>
       <c r="D2" s="252" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="E2" s="252"/>
       <c r="F2" s="252"/>
@@ -26970,7 +27169,7 @@
       <c r="J2" s="252"/>
       <c r="K2" s="252"/>
       <c r="L2" s="253" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="M2" s="253"/>
       <c r="N2" s="10"/>
@@ -27010,21 +27209,21 @@
     <row r="5" spans="1:18" customHeight="1" ht="15">
       <c r="A5" s="10"/>
       <c r="B5" s="235" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C5" s="236"/>
       <c r="D5" s="236"/>
       <c r="E5" s="236"/>
       <c r="F5" s="237"/>
       <c r="G5" s="235" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="H5" s="236"/>
       <c r="I5" s="236"/>
       <c r="J5" s="236"/>
       <c r="K5" s="237"/>
       <c r="L5" s="235" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="M5" s="237"/>
       <c r="N5" s="10"/>
@@ -27039,14 +27238,14 @@
       <c r="E6" s="248"/>
       <c r="F6" s="249"/>
       <c r="G6" s="247">
-        <v>8563214</v>
+        <v>856491</v>
       </c>
       <c r="H6" s="248"/>
       <c r="I6" s="248"/>
       <c r="J6" s="248"/>
       <c r="K6" s="249"/>
       <c r="L6" s="250" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="M6" s="251"/>
       <c r="N6" s="10"/>
@@ -27069,13 +27268,13 @@
       <c r="N7" s="3"/>
       <c r="O7" s="30"/>
       <c r="P7" s="48" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:18" customHeight="1" ht="15">
       <c r="A8" s="13"/>
       <c r="B8" s="137" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="C8" s="138"/>
       <c r="D8" s="138"/>
@@ -27091,7 +27290,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="31"/>
       <c r="P8" s="49" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="Q8" s="29"/>
       <c r="R8" s="31"/>
@@ -27099,7 +27298,7 @@
     <row r="9" spans="1:18" customHeight="1" ht="15">
       <c r="A9" s="13"/>
       <c r="B9" s="93" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="C9" s="140"/>
       <c r="D9" s="141"/>
@@ -27115,7 +27314,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="31"/>
       <c r="P9" s="48" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="Q9" s="29"/>
       <c r="R9" s="31"/>
@@ -27124,7 +27323,7 @@
       <c r="A10" s="13"/>
       <c r="B10" s="93"/>
       <c r="C10" s="144" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D10" s="140"/>
       <c r="E10" s="141"/>
@@ -27139,7 +27338,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="31"/>
       <c r="P10" s="48" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="Q10" s="29"/>
       <c r="R10" s="31"/>
@@ -27147,7 +27346,7 @@
     <row r="11" spans="1:18" customHeight="1" ht="15">
       <c r="A11" s="13"/>
       <c r="B11" s="93" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C11" s="140"/>
       <c r="D11" s="141">
@@ -27172,7 +27371,7 @@
       <c r="A12" s="13"/>
       <c r="B12" s="93"/>
       <c r="C12" s="144" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D12" s="140"/>
       <c r="E12" s="141"/>
@@ -27192,7 +27391,7 @@
     <row r="13" spans="1:18" customHeight="1" ht="15">
       <c r="A13" s="13"/>
       <c r="B13" s="93" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="C13" s="140"/>
       <c r="D13" s="141">
@@ -27217,7 +27416,7 @@
       <c r="A14" s="13"/>
       <c r="B14" s="93"/>
       <c r="C14" s="144" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D14" s="140"/>
       <c r="E14" s="141"/>
@@ -27237,7 +27436,7 @@
     <row r="15" spans="1:18" customHeight="1" ht="15">
       <c r="A15" s="13"/>
       <c r="B15" s="93" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="C15" s="140"/>
       <c r="D15" s="141">
@@ -27262,7 +27461,7 @@
       <c r="A16" s="13"/>
       <c r="B16" s="93"/>
       <c r="C16" s="144" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D16" s="140"/>
       <c r="E16" s="141"/>
@@ -27282,7 +27481,7 @@
     <row r="17" spans="1:18" customHeight="1" ht="15">
       <c r="A17" s="13"/>
       <c r="B17" s="93" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C17" s="140"/>
       <c r="D17" s="141">
@@ -27307,7 +27506,7 @@
       <c r="A18" s="13"/>
       <c r="B18" s="93"/>
       <c r="C18" s="144" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D18" s="140"/>
       <c r="E18" s="141"/>
@@ -27327,7 +27526,7 @@
     <row r="19" spans="1:18" customHeight="1" ht="15">
       <c r="A19" s="13"/>
       <c r="B19" s="93" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="C19" s="140"/>
       <c r="D19" s="141">
@@ -27352,7 +27551,7 @@
       <c r="A20" s="13"/>
       <c r="B20" s="93"/>
       <c r="C20" s="144" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D20" s="140"/>
       <c r="E20" s="141"/>
@@ -27372,7 +27571,7 @@
     <row r="21" spans="1:18" customHeight="1" ht="15">
       <c r="A21" s="13"/>
       <c r="B21" s="145" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="C21" s="146"/>
       <c r="D21" s="147"/>
@@ -27429,7 +27628,7 @@
     <row r="24" spans="1:18" customHeight="1" ht="15">
       <c r="A24" s="13"/>
       <c r="B24" s="137" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C24" s="138"/>
       <c r="D24" s="138"/>
@@ -27450,7 +27649,7 @@
     <row r="25" spans="1:18" customHeight="1" ht="15">
       <c r="A25" s="13"/>
       <c r="B25" s="93" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="C25" s="140"/>
       <c r="D25" s="141"/>
@@ -27472,7 +27671,7 @@
       <c r="A26" s="13"/>
       <c r="B26" s="93"/>
       <c r="C26" s="144" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D26" s="140"/>
       <c r="E26" s="141"/>
@@ -27492,7 +27691,7 @@
     <row r="27" spans="1:18" customHeight="1" ht="15">
       <c r="A27" s="13"/>
       <c r="B27" s="93" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C27" s="140"/>
       <c r="D27" s="141">
@@ -27517,7 +27716,7 @@
       <c r="A28" s="13"/>
       <c r="B28" s="93"/>
       <c r="C28" s="144" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D28" s="140"/>
       <c r="E28" s="141"/>
@@ -27537,7 +27736,7 @@
     <row r="29" spans="1:18" customHeight="1" ht="15">
       <c r="A29" s="13"/>
       <c r="B29" s="93" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="C29" s="140"/>
       <c r="D29" s="141">
@@ -27562,7 +27761,7 @@
       <c r="A30" s="13"/>
       <c r="B30" s="93"/>
       <c r="C30" s="144" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D30" s="140"/>
       <c r="E30" s="141"/>
@@ -27582,7 +27781,7 @@
     <row r="31" spans="1:18" customHeight="1" ht="15">
       <c r="A31" s="13"/>
       <c r="B31" s="93" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="C31" s="140"/>
       <c r="D31" s="141">
@@ -27607,7 +27806,7 @@
       <c r="A32" s="13"/>
       <c r="B32" s="93"/>
       <c r="C32" s="144" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D32" s="140"/>
       <c r="E32" s="141"/>
@@ -27627,7 +27826,7 @@
     <row r="33" spans="1:18" customHeight="1" ht="15">
       <c r="A33" s="13"/>
       <c r="B33" s="93" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C33" s="140"/>
       <c r="D33" s="141">
@@ -27652,7 +27851,7 @@
       <c r="A34" s="13"/>
       <c r="B34" s="93"/>
       <c r="C34" s="144" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D34" s="140"/>
       <c r="E34" s="141"/>
@@ -27672,7 +27871,7 @@
     <row r="35" spans="1:18" customHeight="1" ht="15">
       <c r="A35" s="13"/>
       <c r="B35" s="93" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="C35" s="140"/>
       <c r="D35" s="141">
@@ -27697,7 +27896,7 @@
       <c r="A36" s="13"/>
       <c r="B36" s="93"/>
       <c r="C36" s="144" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D36" s="140"/>
       <c r="E36" s="141"/>
@@ -27717,7 +27916,7 @@
     <row r="37" spans="1:18" customHeight="1" ht="15">
       <c r="A37" s="13"/>
       <c r="B37" s="145" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="C37" s="146"/>
       <c r="D37" s="147"/>
@@ -27774,7 +27973,7 @@
     <row r="40" spans="1:18" customHeight="1" ht="15">
       <c r="A40" s="13"/>
       <c r="B40" s="230" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="C40" s="231"/>
       <c r="D40" s="231"/>
@@ -27795,7 +27994,7 @@
     <row r="41" spans="1:18" customHeight="1" ht="15">
       <c r="A41" s="13"/>
       <c r="B41" s="434" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="C41" s="434"/>
       <c r="D41" s="194"/>
@@ -27817,7 +28016,7 @@
       <c r="A42" s="13"/>
       <c r="B42" s="93"/>
       <c r="C42" s="435" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D42" s="434"/>
       <c r="E42" s="194"/>
@@ -27837,7 +28036,7 @@
     <row r="43" spans="1:18" customHeight="1" ht="15">
       <c r="A43" s="13"/>
       <c r="B43" s="434" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C43" s="434"/>
       <c r="D43" s="194">
@@ -27862,7 +28061,7 @@
       <c r="A44" s="13"/>
       <c r="B44" s="93"/>
       <c r="C44" s="435" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D44" s="434"/>
       <c r="E44" s="194"/>
@@ -27882,7 +28081,7 @@
     <row r="45" spans="1:18" customHeight="1" ht="15">
       <c r="A45" s="13"/>
       <c r="B45" s="434" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="C45" s="434"/>
       <c r="D45" s="194">
@@ -27907,7 +28106,7 @@
       <c r="A46" s="13"/>
       <c r="B46" s="93"/>
       <c r="C46" s="435" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D46" s="434"/>
       <c r="E46" s="194"/>
@@ -27927,7 +28126,7 @@
     <row r="47" spans="1:18" customHeight="1" ht="15">
       <c r="A47" s="13"/>
       <c r="B47" s="434" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="C47" s="434"/>
       <c r="D47" s="194">
@@ -27952,7 +28151,7 @@
       <c r="A48" s="13"/>
       <c r="B48" s="93"/>
       <c r="C48" s="435" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D48" s="434"/>
       <c r="E48" s="194"/>
@@ -27972,7 +28171,7 @@
     <row r="49" spans="1:18" customHeight="1" ht="15">
       <c r="A49" s="13"/>
       <c r="B49" s="434" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C49" s="434"/>
       <c r="D49" s="194">
@@ -27997,7 +28196,7 @@
       <c r="A50" s="13"/>
       <c r="B50" s="93"/>
       <c r="C50" s="435" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D50" s="434"/>
       <c r="E50" s="194"/>
@@ -28017,7 +28216,7 @@
     <row r="51" spans="1:18" customHeight="1" ht="15">
       <c r="A51" s="13"/>
       <c r="B51" s="434" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="C51" s="434"/>
       <c r="D51" s="194">
@@ -28042,7 +28241,7 @@
       <c r="A52" s="13"/>
       <c r="B52" s="93"/>
       <c r="C52" s="435" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D52" s="434"/>
       <c r="E52" s="194"/>
@@ -28062,7 +28261,7 @@
     <row r="53" spans="1:18" customHeight="1" ht="15">
       <c r="A53" s="13"/>
       <c r="B53" s="436" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="C53" s="437"/>
       <c r="D53" s="438"/>

</xml_diff>